<commit_message>
changes to item and list
</commit_message>
<xml_diff>
--- a/documents/bugs/TaskStore Bug List.xlsx
+++ b/documents/bugs/TaskStore Bug List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="337">
   <si>
     <t>Feature</t>
   </si>
@@ -1018,6 +1018,15 @@
   </si>
   <si>
     <t>Remove ID from FieldValue to reduce wire size</t>
+  </si>
+  <si>
+    <t>EF needs the ID as a primary key, and without it, it's hard to figure out new FieldValues vs existing ones</t>
+  </si>
+  <si>
+    <t>DELETE fails against folder</t>
+  </si>
+  <si>
+    <t>It appears that the client sends null for FolderUsers which trips up the service.  The client needs to add FolderUsers</t>
   </si>
 </sst>
 </file>
@@ -1087,8 +1096,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="A1:I173" totalsRowShown="0">
-  <autoFilter ref="A1:I173"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="A1:I174" totalsRowShown="0">
+  <autoFilter ref="A1:I174"/>
   <sortState ref="A2:I157">
     <sortCondition ref="A1:A157"/>
   </sortState>
@@ -1734,10 +1743,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I173"/>
+  <dimension ref="A1:I174"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="A173" sqref="A173"/>
+      <selection activeCell="A175" sqref="A175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5798,7 +5807,36 @@
         <v>1</v>
       </c>
       <c r="G173" t="s">
+        <v>127</v>
+      </c>
+      <c r="H173" t="s">
+        <v>45</v>
+      </c>
+      <c r="I173" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>173</v>
+      </c>
+      <c r="B174" t="s">
+        <v>335</v>
+      </c>
+      <c r="C174" t="s">
+        <v>22</v>
+      </c>
+      <c r="D174">
+        <v>1</v>
+      </c>
+      <c r="F174">
+        <v>1</v>
+      </c>
+      <c r="G174" t="s">
         <v>21</v>
+      </c>
+      <c r="I174" t="s">
+        <v>336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>